<commit_message>
update result  text label
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E45"/>
+  <dimension ref="A2:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>45913.9101290203</v>
+        <v>45913.91012901621</v>
       </c>
       <c r="B38" t="n">
         <v>264</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>45913.91039145063</v>
+        <v>45913.91039144676</v>
       </c>
       <c r="B39" t="n">
         <v>264</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>45913.9106208444</v>
+        <v>45913.91062084491</v>
       </c>
       <c r="B40" t="n">
         <v>660</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>45913.9113326705</v>
+        <v>45913.91133267361</v>
       </c>
       <c r="B41" t="n">
         <v>660</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>45913.91175178665</v>
+        <v>45913.91175178241</v>
       </c>
       <c r="B42" t="n">
         <v>660</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45913.91236648113</v>
+        <v>45913.91236648148</v>
       </c>
       <c r="B43" t="n">
         <v>660</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>45913.91350438834</v>
+        <v>45913.91350438658</v>
       </c>
       <c r="B44" t="n">
         <v>660</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>45913.91387810817</v>
+        <v>45913.91387811342</v>
       </c>
       <c r="B45" t="n">
         <v>660</v>
@@ -1343,6 +1343,69 @@
         </is>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>45913.91664212963</v>
+      </c>
+      <c r="B46" t="n">
+        <v>660</v>
+      </c>
+      <c r="C46" t="n">
+        <v>264</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45913.92082518519</v>
+      </c>
+      <c r="B47" t="n">
+        <v>660</v>
+      </c>
+      <c r="C47" t="n">
+        <v>264</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>45913.921534596</v>
+      </c>
+      <c r="B48" t="n">
+        <v>660</v>
+      </c>
+      <c r="C48" t="n">
+        <v>264</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
         </is>

</xml_diff>

<commit_message>
input time base on wath dog timer or manual
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E48"/>
+  <dimension ref="A2:E52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>45913.921534596</v>
+        <v>45913.92153459491</v>
       </c>
       <c r="B48" t="n">
         <v>660</v>
@@ -1406,6 +1406,90 @@
         </is>
       </c>
       <c r="E48" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>45914.3330212963</v>
+      </c>
+      <c r="B49" t="n">
+        <v>660</v>
+      </c>
+      <c r="C49" t="n">
+        <v>264</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0:0</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>45914.34451471065</v>
+      </c>
+      <c r="B50" t="n">
+        <v>660</v>
+      </c>
+      <c r="C50" t="n">
+        <v>264</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>45914.34880066659</v>
+      </c>
+      <c r="B51" t="n">
+        <v>660</v>
+      </c>
+      <c r="C51" t="n">
+        <v>462</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 462.0 MW/Giảm tải xuống 462.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>45914.34907038009</v>
+      </c>
+      <c r="B52" t="n">
+        <v>660</v>
+      </c>
+      <c r="C52" t="n">
+        <v>264</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
         </is>

</xml_diff>

<commit_message>
add sound alarm for overide load
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E811"/>
+  <dimension ref="A2:E854"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11325,7 +11325,7 @@
     </row>
     <row r="719">
       <c r="A719" s="1" t="n">
-        <v>45914.49244710076</v>
+        <v>45914.49244710648</v>
       </c>
       <c r="B719" t="n">
         <v>264</v>
@@ -11346,7 +11346,7 @@
     </row>
     <row r="720">
       <c r="A720" s="1" t="n">
-        <v>45914.49260667551</v>
+        <v>45914.49260667824</v>
       </c>
       <c r="B720" t="n">
         <v>264</v>
@@ -11652,7 +11652,7 @@
     </row>
     <row r="740">
       <c r="A740" s="1" t="n">
-        <v>45914.49333404485</v>
+        <v>45914.49333403935</v>
       </c>
       <c r="B740" t="n">
         <v>264</v>
@@ -11943,7 +11943,7 @@
     </row>
     <row r="759">
       <c r="A759" s="1" t="n">
-        <v>45914.49444172283</v>
+        <v>45914.49444172454</v>
       </c>
       <c r="B759" t="n">
         <v>660</v>
@@ -12174,7 +12174,7 @@
     </row>
     <row r="774">
       <c r="A774" s="1" t="n">
-        <v>45914.4958113414</v>
+        <v>45914.49581134259</v>
       </c>
       <c r="B774" t="n">
         <v>660</v>
@@ -12465,7 +12465,7 @@
     </row>
     <row r="793">
       <c r="A793" s="1" t="n">
-        <v>45914.49678841136</v>
+        <v>45914.49678841436</v>
       </c>
       <c r="B793" t="n">
         <v>264</v>
@@ -12749,6 +12749,681 @@
         <v>264</v>
       </c>
       <c r="C811" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="1" t="n">
+        <v>45914.5060709375</v>
+      </c>
+      <c r="B812" t="n">
+        <v>264</v>
+      </c>
+      <c r="C812" t="n">
+        <v>660</v>
+      </c>
+      <c r="D812" t="inlineStr">
+        <is>
+          <t>12:08</t>
+        </is>
+      </c>
+      <c r="E812" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="1" t="n">
+        <v>45914.50642701389</v>
+      </c>
+      <c r="B813" t="n">
+        <v>264</v>
+      </c>
+      <c r="C813" t="n">
+        <v>660</v>
+      </c>
+      <c r="D813" t="inlineStr">
+        <is>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="E813" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="1" t="n">
+        <v>45914.50908366948</v>
+      </c>
+      <c r="B814" t="n">
+        <v>264</v>
+      </c>
+      <c r="C814" t="n">
+        <v>660</v>
+      </c>
+      <c r="D814" t="inlineStr">
+        <is>
+          <t>23:12</t>
+        </is>
+      </c>
+      <c r="E814" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" s="1" t="n">
+        <v>45914.50930866507</v>
+      </c>
+      <c r="B815" t="n">
+        <v>264</v>
+      </c>
+      <c r="C815" t="n">
+        <v>600</v>
+      </c>
+      <c r="D815" t="inlineStr">
+        <is>
+          <t>12:13</t>
+        </is>
+      </c>
+      <c r="E815" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:46:00</t>
+        </is>
+      </c>
+      <c r="B816" t="n">
+        <v>429</v>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:47:00</t>
+        </is>
+      </c>
+      <c r="B817" t="n">
+        <v>442.2</v>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:48:00</t>
+        </is>
+      </c>
+      <c r="B818" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:49:00</t>
+        </is>
+      </c>
+      <c r="B819" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:50:00</t>
+        </is>
+      </c>
+      <c r="B820" t="n">
+        <v>481.8</v>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:51:00</t>
+        </is>
+      </c>
+      <c r="B821" t="n">
+        <v>494.9999999999999</v>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:52:00</t>
+        </is>
+      </c>
+      <c r="B822" t="n">
+        <v>508.1999999999999</v>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:53:00</t>
+        </is>
+      </c>
+      <c r="B823" t="n">
+        <v>521.4</v>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:54:00</t>
+        </is>
+      </c>
+      <c r="B824" t="n">
+        <v>534.6</v>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:55:00</t>
+        </is>
+      </c>
+      <c r="B825" t="n">
+        <v>547.8000000000001</v>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:56:00</t>
+        </is>
+      </c>
+      <c r="B826" t="n">
+        <v>561.0000000000001</v>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:57:00</t>
+        </is>
+      </c>
+      <c r="B827" t="n">
+        <v>574.2000000000002</v>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:58:00</t>
+        </is>
+      </c>
+      <c r="B828" t="n">
+        <v>587.4000000000002</v>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>2025-09-14 12:59:00</t>
+        </is>
+      </c>
+      <c r="B829" t="n">
+        <v>600.6000000000003</v>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:00:00</t>
+        </is>
+      </c>
+      <c r="B830" t="n">
+        <v>613.8000000000003</v>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:01:00</t>
+        </is>
+      </c>
+      <c r="B831" t="n">
+        <v>627.0000000000003</v>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:02:00</t>
+        </is>
+      </c>
+      <c r="B832" t="n">
+        <v>640.2000000000004</v>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:03:00</t>
+        </is>
+      </c>
+      <c r="B833" t="n">
+        <v>653.4000000000004</v>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:04:00</t>
+        </is>
+      </c>
+      <c r="B834" t="n">
+        <v>660</v>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" s="1" t="n">
+        <v>45914.50971411171</v>
+      </c>
+      <c r="B835" t="n">
+        <v>264</v>
+      </c>
+      <c r="C835" t="n">
+        <v>600</v>
+      </c>
+      <c r="D835" t="inlineStr">
+        <is>
+          <t>23:13</t>
+        </is>
+      </c>
+      <c r="E835" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:46:00</t>
+        </is>
+      </c>
+      <c r="B836" t="n">
+        <v>429</v>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:47:00</t>
+        </is>
+      </c>
+      <c r="B837" t="n">
+        <v>442.2</v>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:48:00</t>
+        </is>
+      </c>
+      <c r="B838" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:49:00</t>
+        </is>
+      </c>
+      <c r="B839" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:50:00</t>
+        </is>
+      </c>
+      <c r="B840" t="n">
+        <v>481.8</v>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:51:00</t>
+        </is>
+      </c>
+      <c r="B841" t="n">
+        <v>494.9999999999999</v>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:52:00</t>
+        </is>
+      </c>
+      <c r="B842" t="n">
+        <v>508.1999999999999</v>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:53:00</t>
+        </is>
+      </c>
+      <c r="B843" t="n">
+        <v>521.4</v>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:54:00</t>
+        </is>
+      </c>
+      <c r="B844" t="n">
+        <v>534.6</v>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:55:00</t>
+        </is>
+      </c>
+      <c r="B845" t="n">
+        <v>547.8000000000001</v>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:56:00</t>
+        </is>
+      </c>
+      <c r="B846" t="n">
+        <v>561.0000000000001</v>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:57:00</t>
+        </is>
+      </c>
+      <c r="B847" t="n">
+        <v>574.2000000000002</v>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:58:00</t>
+        </is>
+      </c>
+      <c r="B848" t="n">
+        <v>587.4000000000002</v>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>2025-09-14 23:59:00</t>
+        </is>
+      </c>
+      <c r="B849" t="n">
+        <v>600.6000000000003</v>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="B850" t="n">
+        <v>613.8000000000003</v>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:01:00</t>
+        </is>
+      </c>
+      <c r="B851" t="n">
+        <v>627.0000000000003</v>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:02:00</t>
+        </is>
+      </c>
+      <c r="B852" t="n">
+        <v>640.2000000000004</v>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:03:00</t>
+        </is>
+      </c>
+      <c r="B853" t="n">
+        <v>653.4000000000004</v>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:04:00</t>
+        </is>
+      </c>
+      <c r="B854" t="n">
+        <v>660</v>
+      </c>
+      <c r="C854" t="inlineStr">
         <is>
           <t>ramp</t>
         </is>

</xml_diff>

<commit_message>
Add link plot funtion
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E854"/>
+  <dimension ref="A2:E1144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12798,7 +12798,7 @@
     </row>
     <row r="814">
       <c r="A814" s="1" t="n">
-        <v>45914.50908366948</v>
+        <v>45914.50908366899</v>
       </c>
       <c r="B814" t="n">
         <v>264</v>
@@ -12819,7 +12819,7 @@
     </row>
     <row r="815">
       <c r="A815" s="1" t="n">
-        <v>45914.50930866507</v>
+        <v>45914.50930866898</v>
       </c>
       <c r="B815" t="n">
         <v>264</v>
@@ -13125,7 +13125,7 @@
     </row>
     <row r="835">
       <c r="A835" s="1" t="n">
-        <v>45914.50971411171</v>
+        <v>45914.5097141088</v>
       </c>
       <c r="B835" t="n">
         <v>264</v>
@@ -13424,6 +13424,4464 @@
         <v>660</v>
       </c>
       <c r="C854" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="1" t="n">
+        <v>45914.51505253472</v>
+      </c>
+      <c r="B855" t="n">
+        <v>264</v>
+      </c>
+      <c r="C855" t="n">
+        <v>660</v>
+      </c>
+      <c r="D855" t="inlineStr">
+        <is>
+          <t>23:30</t>
+        </is>
+      </c>
+      <c r="E855" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="1" t="n">
+        <v>45914.5152600463</v>
+      </c>
+      <c r="B856" t="n">
+        <v>264</v>
+      </c>
+      <c r="C856" t="n">
+        <v>660</v>
+      </c>
+      <c r="D856" t="inlineStr">
+        <is>
+          <t>23:10</t>
+        </is>
+      </c>
+      <c r="E856" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="1" t="n">
+        <v>45914.51542164352</v>
+      </c>
+      <c r="B857" t="n">
+        <v>264</v>
+      </c>
+      <c r="C857" t="n">
+        <v>660</v>
+      </c>
+      <c r="D857" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E857" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:18:00</t>
+        </is>
+      </c>
+      <c r="B858" t="n">
+        <v>429</v>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:19:00</t>
+        </is>
+      </c>
+      <c r="B859" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:20:00</t>
+        </is>
+      </c>
+      <c r="B860" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:21:00</t>
+        </is>
+      </c>
+      <c r="B861" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:22:00</t>
+        </is>
+      </c>
+      <c r="B862" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:23:00</t>
+        </is>
+      </c>
+      <c r="B863" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:24:00</t>
+        </is>
+      </c>
+      <c r="B864" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:25:00</t>
+        </is>
+      </c>
+      <c r="B865" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:26:00</t>
+        </is>
+      </c>
+      <c r="B866" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:27:00</t>
+        </is>
+      </c>
+      <c r="B867" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:28:00</t>
+        </is>
+      </c>
+      <c r="B868" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:29:00</t>
+        </is>
+      </c>
+      <c r="B869" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:30:00</t>
+        </is>
+      </c>
+      <c r="B870" t="n">
+        <v>297</v>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:31:00</t>
+        </is>
+      </c>
+      <c r="B871" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:32:00</t>
+        </is>
+      </c>
+      <c r="B872" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:33:00</t>
+        </is>
+      </c>
+      <c r="B873" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:34:00</t>
+        </is>
+      </c>
+      <c r="B874" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>2025-09-15 00:35:00</t>
+        </is>
+      </c>
+      <c r="B875" t="n">
+        <v>264</v>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="1" t="n">
+        <v>45914.52121304398</v>
+      </c>
+      <c r="B876" t="n">
+        <v>264</v>
+      </c>
+      <c r="C876" t="n">
+        <v>600</v>
+      </c>
+      <c r="D876" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="E876" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:48:00</t>
+        </is>
+      </c>
+      <c r="B877" t="n">
+        <v>429</v>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:49:00</t>
+        </is>
+      </c>
+      <c r="B878" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:50:00</t>
+        </is>
+      </c>
+      <c r="B879" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:51:00</t>
+        </is>
+      </c>
+      <c r="B880" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:52:00</t>
+        </is>
+      </c>
+      <c r="B881" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:53:00</t>
+        </is>
+      </c>
+      <c r="B882" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:54:00</t>
+        </is>
+      </c>
+      <c r="B883" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:55:00</t>
+        </is>
+      </c>
+      <c r="B884" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:56:00</t>
+        </is>
+      </c>
+      <c r="B885" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:57:00</t>
+        </is>
+      </c>
+      <c r="B886" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:58:00</t>
+        </is>
+      </c>
+      <c r="B887" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:59:00</t>
+        </is>
+      </c>
+      <c r="B888" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:00:00</t>
+        </is>
+      </c>
+      <c r="B889" t="n">
+        <v>297</v>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:01:00</t>
+        </is>
+      </c>
+      <c r="B890" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:02:00</t>
+        </is>
+      </c>
+      <c r="B891" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:03:00</t>
+        </is>
+      </c>
+      <c r="B892" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:04:00</t>
+        </is>
+      </c>
+      <c r="B893" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:05:00</t>
+        </is>
+      </c>
+      <c r="B894" t="n">
+        <v>264</v>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="1" t="n">
+        <v>45914.52444666667</v>
+      </c>
+      <c r="B895" t="n">
+        <v>264</v>
+      </c>
+      <c r="C895" t="n">
+        <v>600</v>
+      </c>
+      <c r="D895" t="inlineStr">
+        <is>
+          <t>12:35</t>
+        </is>
+      </c>
+      <c r="E895" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:53:00</t>
+        </is>
+      </c>
+      <c r="B896" t="n">
+        <v>429</v>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:54:00</t>
+        </is>
+      </c>
+      <c r="B897" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:55:00</t>
+        </is>
+      </c>
+      <c r="B898" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:56:00</t>
+        </is>
+      </c>
+      <c r="B899" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:57:00</t>
+        </is>
+      </c>
+      <c r="B900" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:58:00</t>
+        </is>
+      </c>
+      <c r="B901" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:59:00</t>
+        </is>
+      </c>
+      <c r="B902" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:00:00</t>
+        </is>
+      </c>
+      <c r="B903" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:01:00</t>
+        </is>
+      </c>
+      <c r="B904" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:02:00</t>
+        </is>
+      </c>
+      <c r="B905" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:03:00</t>
+        </is>
+      </c>
+      <c r="B906" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:04:00</t>
+        </is>
+      </c>
+      <c r="B907" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:05:00</t>
+        </is>
+      </c>
+      <c r="B908" t="n">
+        <v>297</v>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:06:00</t>
+        </is>
+      </c>
+      <c r="B909" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:07:00</t>
+        </is>
+      </c>
+      <c r="B910" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:08:00</t>
+        </is>
+      </c>
+      <c r="B911" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:09:00</t>
+        </is>
+      </c>
+      <c r="B912" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:10:00</t>
+        </is>
+      </c>
+      <c r="B913" t="n">
+        <v>264</v>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="1" t="n">
+        <v>45914.53543868056</v>
+      </c>
+      <c r="B914" t="n">
+        <v>264</v>
+      </c>
+      <c r="C914" t="n">
+        <v>600</v>
+      </c>
+      <c r="D914" t="inlineStr">
+        <is>
+          <t>12:51</t>
+        </is>
+      </c>
+      <c r="E914" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:09:00</t>
+        </is>
+      </c>
+      <c r="B915" t="n">
+        <v>429</v>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:10:00</t>
+        </is>
+      </c>
+      <c r="B916" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:11:00</t>
+        </is>
+      </c>
+      <c r="B917" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:12:00</t>
+        </is>
+      </c>
+      <c r="B918" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:13:00</t>
+        </is>
+      </c>
+      <c r="B919" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:14:00</t>
+        </is>
+      </c>
+      <c r="B920" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:15:00</t>
+        </is>
+      </c>
+      <c r="B921" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:16:00</t>
+        </is>
+      </c>
+      <c r="B922" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:17:00</t>
+        </is>
+      </c>
+      <c r="B923" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:18:00</t>
+        </is>
+      </c>
+      <c r="B924" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:19:00</t>
+        </is>
+      </c>
+      <c r="B925" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:20:00</t>
+        </is>
+      </c>
+      <c r="B926" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:21:00</t>
+        </is>
+      </c>
+      <c r="B927" t="n">
+        <v>297</v>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:22:00</t>
+        </is>
+      </c>
+      <c r="B928" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:23:00</t>
+        </is>
+      </c>
+      <c r="B929" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:24:00</t>
+        </is>
+      </c>
+      <c r="B930" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:25:00</t>
+        </is>
+      </c>
+      <c r="B931" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:26:00</t>
+        </is>
+      </c>
+      <c r="B932" t="n">
+        <v>264</v>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="1" t="n">
+        <v>45914.53939133102</v>
+      </c>
+      <c r="B933" t="n">
+        <v>264</v>
+      </c>
+      <c r="C933" t="n">
+        <v>660</v>
+      </c>
+      <c r="D933" t="inlineStr">
+        <is>
+          <t>12:56</t>
+        </is>
+      </c>
+      <c r="E933" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:14:00</t>
+        </is>
+      </c>
+      <c r="B934" t="n">
+        <v>429</v>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:15:00</t>
+        </is>
+      </c>
+      <c r="B935" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:16:00</t>
+        </is>
+      </c>
+      <c r="B936" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:17:00</t>
+        </is>
+      </c>
+      <c r="B937" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:18:00</t>
+        </is>
+      </c>
+      <c r="B938" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:19:00</t>
+        </is>
+      </c>
+      <c r="B939" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:20:00</t>
+        </is>
+      </c>
+      <c r="B940" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:21:00</t>
+        </is>
+      </c>
+      <c r="B941" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:22:00</t>
+        </is>
+      </c>
+      <c r="B942" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:23:00</t>
+        </is>
+      </c>
+      <c r="B943" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:24:00</t>
+        </is>
+      </c>
+      <c r="B944" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:25:00</t>
+        </is>
+      </c>
+      <c r="B945" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:26:00</t>
+        </is>
+      </c>
+      <c r="B946" t="n">
+        <v>297</v>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:27:00</t>
+        </is>
+      </c>
+      <c r="B947" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:28:00</t>
+        </is>
+      </c>
+      <c r="B948" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:29:00</t>
+        </is>
+      </c>
+      <c r="B949" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:30:00</t>
+        </is>
+      </c>
+      <c r="B950" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:31:00</t>
+        </is>
+      </c>
+      <c r="B951" t="n">
+        <v>264</v>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" s="1" t="n">
+        <v>45914.53989724537</v>
+      </c>
+      <c r="B952" t="n">
+        <v>264</v>
+      </c>
+      <c r="C952" t="n">
+        <v>660</v>
+      </c>
+      <c r="D952" t="inlineStr">
+        <is>
+          <t>12:57</t>
+        </is>
+      </c>
+      <c r="E952" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:15:00</t>
+        </is>
+      </c>
+      <c r="B953" t="n">
+        <v>429</v>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:16:00</t>
+        </is>
+      </c>
+      <c r="B954" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:17:00</t>
+        </is>
+      </c>
+      <c r="B955" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:18:00</t>
+        </is>
+      </c>
+      <c r="B956" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:19:00</t>
+        </is>
+      </c>
+      <c r="B957" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:20:00</t>
+        </is>
+      </c>
+      <c r="B958" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:21:00</t>
+        </is>
+      </c>
+      <c r="B959" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:22:00</t>
+        </is>
+      </c>
+      <c r="B960" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:23:00</t>
+        </is>
+      </c>
+      <c r="B961" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:24:00</t>
+        </is>
+      </c>
+      <c r="B962" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:25:00</t>
+        </is>
+      </c>
+      <c r="B963" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:26:00</t>
+        </is>
+      </c>
+      <c r="B964" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:27:00</t>
+        </is>
+      </c>
+      <c r="B965" t="n">
+        <v>297</v>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:28:00</t>
+        </is>
+      </c>
+      <c r="B966" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:29:00</t>
+        </is>
+      </c>
+      <c r="B967" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:30:00</t>
+        </is>
+      </c>
+      <c r="B968" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:31:00</t>
+        </is>
+      </c>
+      <c r="B969" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:32:00</t>
+        </is>
+      </c>
+      <c r="B970" t="n">
+        <v>264</v>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" s="1" t="n">
+        <v>45914.54083400463</v>
+      </c>
+      <c r="B971" t="n">
+        <v>264</v>
+      </c>
+      <c r="C971" t="n">
+        <v>500</v>
+      </c>
+      <c r="D971" t="inlineStr">
+        <is>
+          <t>12:58</t>
+        </is>
+      </c>
+      <c r="E971" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 500.0 MW/Tăng tải lên 500.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:31:00</t>
+        </is>
+      </c>
+      <c r="B972" t="n">
+        <v>429</v>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:32:00</t>
+        </is>
+      </c>
+      <c r="B973" t="n">
+        <v>442.2</v>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:33:00</t>
+        </is>
+      </c>
+      <c r="B974" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:34:00</t>
+        </is>
+      </c>
+      <c r="B975" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:35:00</t>
+        </is>
+      </c>
+      <c r="B976" t="n">
+        <v>481.8</v>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:36:00</t>
+        </is>
+      </c>
+      <c r="B977" t="n">
+        <v>494.9999999999999</v>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:37:00</t>
+        </is>
+      </c>
+      <c r="B978" t="n">
+        <v>508.1999999999999</v>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:38:00</t>
+        </is>
+      </c>
+      <c r="B979" t="n">
+        <v>521.4</v>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:39:00</t>
+        </is>
+      </c>
+      <c r="B980" t="n">
+        <v>534.6</v>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:40:00</t>
+        </is>
+      </c>
+      <c r="B981" t="n">
+        <v>547.8000000000001</v>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:41:00</t>
+        </is>
+      </c>
+      <c r="B982" t="n">
+        <v>561.0000000000001</v>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:42:00</t>
+        </is>
+      </c>
+      <c r="B983" t="n">
+        <v>574.2000000000002</v>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:43:00</t>
+        </is>
+      </c>
+      <c r="B984" t="n">
+        <v>587.4000000000002</v>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:44:00</t>
+        </is>
+      </c>
+      <c r="B985" t="n">
+        <v>600.6000000000003</v>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:45:00</t>
+        </is>
+      </c>
+      <c r="B986" t="n">
+        <v>613.8000000000003</v>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:46:00</t>
+        </is>
+      </c>
+      <c r="B987" t="n">
+        <v>627.0000000000003</v>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:47:00</t>
+        </is>
+      </c>
+      <c r="B988" t="n">
+        <v>640.2000000000004</v>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:48:00</t>
+        </is>
+      </c>
+      <c r="B989" t="n">
+        <v>653.4000000000004</v>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:49:00</t>
+        </is>
+      </c>
+      <c r="B990" t="n">
+        <v>660</v>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="1" t="n">
+        <v>45914.5422284375</v>
+      </c>
+      <c r="B991" t="n">
+        <v>264</v>
+      </c>
+      <c r="C991" t="n">
+        <v>660</v>
+      </c>
+      <c r="D991" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="E991" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:18:00</t>
+        </is>
+      </c>
+      <c r="B992" t="n">
+        <v>429</v>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:19:00</t>
+        </is>
+      </c>
+      <c r="B993" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:20:00</t>
+        </is>
+      </c>
+      <c r="B994" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:21:00</t>
+        </is>
+      </c>
+      <c r="B995" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:22:00</t>
+        </is>
+      </c>
+      <c r="B996" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:23:00</t>
+        </is>
+      </c>
+      <c r="B997" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:24:00</t>
+        </is>
+      </c>
+      <c r="B998" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:25:00</t>
+        </is>
+      </c>
+      <c r="B999" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:26:00</t>
+        </is>
+      </c>
+      <c r="B1000" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:27:00</t>
+        </is>
+      </c>
+      <c r="B1001" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:28:00</t>
+        </is>
+      </c>
+      <c r="B1002" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:29:00</t>
+        </is>
+      </c>
+      <c r="B1003" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:30:00</t>
+        </is>
+      </c>
+      <c r="B1004" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:31:00</t>
+        </is>
+      </c>
+      <c r="B1005" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:32:00</t>
+        </is>
+      </c>
+      <c r="B1006" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:33:00</t>
+        </is>
+      </c>
+      <c r="B1007" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:34:00</t>
+        </is>
+      </c>
+      <c r="B1008" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:35:00</t>
+        </is>
+      </c>
+      <c r="B1009" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="1" t="n">
+        <v>45914.54392385417</v>
+      </c>
+      <c r="B1010" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1010" t="n">
+        <v>660</v>
+      </c>
+      <c r="D1010" t="inlineStr">
+        <is>
+          <t>13:03</t>
+        </is>
+      </c>
+      <c r="E1010" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="1" t="n">
+        <v>45914.54881659722</v>
+      </c>
+      <c r="B1011" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1011" t="n">
+        <v>660</v>
+      </c>
+      <c r="D1011" t="inlineStr">
+        <is>
+          <t>13:10</t>
+        </is>
+      </c>
+      <c r="E1011" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:28:00</t>
+        </is>
+      </c>
+      <c r="B1012" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:29:00</t>
+        </is>
+      </c>
+      <c r="B1013" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:30:00</t>
+        </is>
+      </c>
+      <c r="B1014" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:31:00</t>
+        </is>
+      </c>
+      <c r="B1015" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:32:00</t>
+        </is>
+      </c>
+      <c r="B1016" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:33:00</t>
+        </is>
+      </c>
+      <c r="B1017" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:34:00</t>
+        </is>
+      </c>
+      <c r="B1018" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:35:00</t>
+        </is>
+      </c>
+      <c r="B1019" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:36:00</t>
+        </is>
+      </c>
+      <c r="B1020" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:37:00</t>
+        </is>
+      </c>
+      <c r="B1021" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:38:00</t>
+        </is>
+      </c>
+      <c r="B1022" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:39:00</t>
+        </is>
+      </c>
+      <c r="B1023" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:40:00</t>
+        </is>
+      </c>
+      <c r="B1024" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:41:00</t>
+        </is>
+      </c>
+      <c r="B1025" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:42:00</t>
+        </is>
+      </c>
+      <c r="B1026" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:43:00</t>
+        </is>
+      </c>
+      <c r="B1027" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:44:00</t>
+        </is>
+      </c>
+      <c r="B1028" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:45:00</t>
+        </is>
+      </c>
+      <c r="B1029" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" s="1" t="n">
+        <v>45914.55190916666</v>
+      </c>
+      <c r="B1030" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1030" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1030" t="inlineStr">
+        <is>
+          <t>13:14</t>
+        </is>
+      </c>
+      <c r="E1030" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:32:00</t>
+        </is>
+      </c>
+      <c r="B1031" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:33:00</t>
+        </is>
+      </c>
+      <c r="B1032" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:34:00</t>
+        </is>
+      </c>
+      <c r="B1033" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:35:00</t>
+        </is>
+      </c>
+      <c r="B1034" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:36:00</t>
+        </is>
+      </c>
+      <c r="B1035" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:37:00</t>
+        </is>
+      </c>
+      <c r="B1036" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:38:00</t>
+        </is>
+      </c>
+      <c r="B1037" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:39:00</t>
+        </is>
+      </c>
+      <c r="B1038" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:40:00</t>
+        </is>
+      </c>
+      <c r="B1039" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:41:00</t>
+        </is>
+      </c>
+      <c r="B1040" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:42:00</t>
+        </is>
+      </c>
+      <c r="B1041" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:43:00</t>
+        </is>
+      </c>
+      <c r="B1042" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:44:00</t>
+        </is>
+      </c>
+      <c r="B1043" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:45:00</t>
+        </is>
+      </c>
+      <c r="B1044" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:46:00</t>
+        </is>
+      </c>
+      <c r="B1045" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:47:00</t>
+        </is>
+      </c>
+      <c r="B1046" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:48:00</t>
+        </is>
+      </c>
+      <c r="B1047" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:49:00</t>
+        </is>
+      </c>
+      <c r="B1048" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" s="1" t="n">
+        <v>45914.55292201389</v>
+      </c>
+      <c r="B1049" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1049" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1049" t="inlineStr">
+        <is>
+          <t>13:16</t>
+        </is>
+      </c>
+      <c r="E1049" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:49:00</t>
+        </is>
+      </c>
+      <c r="B1050" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:50:00</t>
+        </is>
+      </c>
+      <c r="B1051" t="n">
+        <v>442.2</v>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:51:00</t>
+        </is>
+      </c>
+      <c r="B1052" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:52:00</t>
+        </is>
+      </c>
+      <c r="B1053" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:53:00</t>
+        </is>
+      </c>
+      <c r="B1054" t="n">
+        <v>481.8</v>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:54:00</t>
+        </is>
+      </c>
+      <c r="B1055" t="n">
+        <v>494.9999999999999</v>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:55:00</t>
+        </is>
+      </c>
+      <c r="B1056" t="n">
+        <v>508.1999999999999</v>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:56:00</t>
+        </is>
+      </c>
+      <c r="B1057" t="n">
+        <v>521.4</v>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:57:00</t>
+        </is>
+      </c>
+      <c r="B1058" t="n">
+        <v>534.6</v>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:58:00</t>
+        </is>
+      </c>
+      <c r="B1059" t="n">
+        <v>547.8000000000001</v>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>2025-09-14 13:59:00</t>
+        </is>
+      </c>
+      <c r="B1060" t="n">
+        <v>561.0000000000001</v>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:00:00</t>
+        </is>
+      </c>
+      <c r="B1061" t="n">
+        <v>574.2000000000002</v>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:01:00</t>
+        </is>
+      </c>
+      <c r="B1062" t="n">
+        <v>587.4000000000002</v>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:02:00</t>
+        </is>
+      </c>
+      <c r="B1063" t="n">
+        <v>600.6000000000003</v>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:03:00</t>
+        </is>
+      </c>
+      <c r="B1064" t="n">
+        <v>613.8000000000003</v>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:04:00</t>
+        </is>
+      </c>
+      <c r="B1065" t="n">
+        <v>627.0000000000003</v>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:05:00</t>
+        </is>
+      </c>
+      <c r="B1066" t="n">
+        <v>640.2000000000004</v>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:06:00</t>
+        </is>
+      </c>
+      <c r="B1067" t="n">
+        <v>653.4000000000004</v>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:07:00</t>
+        </is>
+      </c>
+      <c r="B1068" t="n">
+        <v>660</v>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" s="1" t="n">
+        <v>45914.55392931713</v>
+      </c>
+      <c r="B1069" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1069" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1069" t="inlineStr">
+        <is>
+          <t>13:17</t>
+        </is>
+      </c>
+      <c r="E1069" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:35:00</t>
+        </is>
+      </c>
+      <c r="B1070" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:36:00</t>
+        </is>
+      </c>
+      <c r="B1071" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:37:00</t>
+        </is>
+      </c>
+      <c r="B1072" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:38:00</t>
+        </is>
+      </c>
+      <c r="B1073" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:39:00</t>
+        </is>
+      </c>
+      <c r="B1074" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:40:00</t>
+        </is>
+      </c>
+      <c r="B1075" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:41:00</t>
+        </is>
+      </c>
+      <c r="B1076" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:42:00</t>
+        </is>
+      </c>
+      <c r="B1077" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:43:00</t>
+        </is>
+      </c>
+      <c r="B1078" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:44:00</t>
+        </is>
+      </c>
+      <c r="B1079" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:45:00</t>
+        </is>
+      </c>
+      <c r="B1080" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:46:00</t>
+        </is>
+      </c>
+      <c r="B1081" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:47:00</t>
+        </is>
+      </c>
+      <c r="B1082" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:48:00</t>
+        </is>
+      </c>
+      <c r="B1083" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:49:00</t>
+        </is>
+      </c>
+      <c r="B1084" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:50:00</t>
+        </is>
+      </c>
+      <c r="B1085" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:51:00</t>
+        </is>
+      </c>
+      <c r="B1086" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:52:00</t>
+        </is>
+      </c>
+      <c r="B1087" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" s="1" t="n">
+        <v>45914.55831707176</v>
+      </c>
+      <c r="B1088" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1088" t="n">
+        <v>556</v>
+      </c>
+      <c r="D1088" t="inlineStr">
+        <is>
+          <t>13:23</t>
+        </is>
+      </c>
+      <c r="E1088" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 556.0 MW/Tăng tải lên 556.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:41:00</t>
+        </is>
+      </c>
+      <c r="B1089" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:42:00</t>
+        </is>
+      </c>
+      <c r="B1090" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:43:00</t>
+        </is>
+      </c>
+      <c r="B1091" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:44:00</t>
+        </is>
+      </c>
+      <c r="B1092" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:45:00</t>
+        </is>
+      </c>
+      <c r="B1093" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:46:00</t>
+        </is>
+      </c>
+      <c r="B1094" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:47:00</t>
+        </is>
+      </c>
+      <c r="B1095" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:48:00</t>
+        </is>
+      </c>
+      <c r="B1096" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:49:00</t>
+        </is>
+      </c>
+      <c r="B1097" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:50:00</t>
+        </is>
+      </c>
+      <c r="B1098" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:51:00</t>
+        </is>
+      </c>
+      <c r="B1099" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:52:00</t>
+        </is>
+      </c>
+      <c r="B1100" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:53:00</t>
+        </is>
+      </c>
+      <c r="B1101" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:54:00</t>
+        </is>
+      </c>
+      <c r="B1102" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:55:00</t>
+        </is>
+      </c>
+      <c r="B1103" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:56:00</t>
+        </is>
+      </c>
+      <c r="B1104" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:57:00</t>
+        </is>
+      </c>
+      <c r="B1105" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:58:00</t>
+        </is>
+      </c>
+      <c r="B1106" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" s="1" t="n">
+        <v>45914.56013976852</v>
+      </c>
+      <c r="B1107" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1107" t="n">
+        <v>654</v>
+      </c>
+      <c r="D1107" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="E1107" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 654.0 MW/Tăng tải lên 654.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:44:00</t>
+        </is>
+      </c>
+      <c r="B1108" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:45:00</t>
+        </is>
+      </c>
+      <c r="B1109" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:46:00</t>
+        </is>
+      </c>
+      <c r="B1110" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:47:00</t>
+        </is>
+      </c>
+      <c r="B1111" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:48:00</t>
+        </is>
+      </c>
+      <c r="B1112" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:49:00</t>
+        </is>
+      </c>
+      <c r="B1113" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:50:00</t>
+        </is>
+      </c>
+      <c r="B1114" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:51:00</t>
+        </is>
+      </c>
+      <c r="B1115" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:52:00</t>
+        </is>
+      </c>
+      <c r="B1116" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:53:00</t>
+        </is>
+      </c>
+      <c r="B1117" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:54:00</t>
+        </is>
+      </c>
+      <c r="B1118" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:55:00</t>
+        </is>
+      </c>
+      <c r="B1119" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:56:00</t>
+        </is>
+      </c>
+      <c r="B1120" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:57:00</t>
+        </is>
+      </c>
+      <c r="B1121" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:58:00</t>
+        </is>
+      </c>
+      <c r="B1122" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:59:00</t>
+        </is>
+      </c>
+      <c r="B1123" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:00:00</t>
+        </is>
+      </c>
+      <c r="B1124" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:01:00</t>
+        </is>
+      </c>
+      <c r="B1125" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" s="1" t="n">
+        <v>45914.56159087654</v>
+      </c>
+      <c r="B1126" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1126" t="n">
+        <v>555</v>
+      </c>
+      <c r="D1126" t="inlineStr">
+        <is>
+          <t>13:28</t>
+        </is>
+      </c>
+      <c r="E1126" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 555.0 MW/Tăng tải lên 555.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:46:00</t>
+        </is>
+      </c>
+      <c r="B1127" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:47:00</t>
+        </is>
+      </c>
+      <c r="B1128" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:48:00</t>
+        </is>
+      </c>
+      <c r="B1129" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:49:00</t>
+        </is>
+      </c>
+      <c r="B1130" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:50:00</t>
+        </is>
+      </c>
+      <c r="B1131" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:51:00</t>
+        </is>
+      </c>
+      <c r="B1132" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:52:00</t>
+        </is>
+      </c>
+      <c r="B1133" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:53:00</t>
+        </is>
+      </c>
+      <c r="B1134" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:54:00</t>
+        </is>
+      </c>
+      <c r="B1135" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:55:00</t>
+        </is>
+      </c>
+      <c r="B1136" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:56:00</t>
+        </is>
+      </c>
+      <c r="B1137" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:57:00</t>
+        </is>
+      </c>
+      <c r="B1138" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:58:00</t>
+        </is>
+      </c>
+      <c r="B1139" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:59:00</t>
+        </is>
+      </c>
+      <c r="B1140" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:00:00</t>
+        </is>
+      </c>
+      <c r="B1141" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:01:00</t>
+        </is>
+      </c>
+      <c r="B1142" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:02:00</t>
+        </is>
+      </c>
+      <c r="B1143" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:03:00</t>
+        </is>
+      </c>
+      <c r="B1144" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1144" t="inlineStr">
         <is>
           <t>ramp</t>
         </is>

</xml_diff>

<commit_message>
update to have live time for hold ad them lenh
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E1144"/>
+  <dimension ref="A2:E1264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17598,7 +17598,7 @@
     </row>
     <row r="1126">
       <c r="A1126" s="1" t="n">
-        <v>45914.56159087654</v>
+        <v>45914.56159087963</v>
       </c>
       <c r="B1126" t="n">
         <v>264</v>
@@ -17882,6 +17882,1866 @@
         <v>264</v>
       </c>
       <c r="C1144" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" s="1" t="n">
+        <v>45914.57733601852</v>
+      </c>
+      <c r="B1145" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1145" t="n">
+        <v>550</v>
+      </c>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="E1145" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 550.0 MW/Tăng tải lên 550.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:09:00</t>
+        </is>
+      </c>
+      <c r="B1146" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:10:00</t>
+        </is>
+      </c>
+      <c r="B1147" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:11:00</t>
+        </is>
+      </c>
+      <c r="B1148" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:12:00</t>
+        </is>
+      </c>
+      <c r="B1149" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:13:00</t>
+        </is>
+      </c>
+      <c r="B1150" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:14:00</t>
+        </is>
+      </c>
+      <c r="B1151" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:15:00</t>
+        </is>
+      </c>
+      <c r="B1152" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:16:00</t>
+        </is>
+      </c>
+      <c r="B1153" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:17:00</t>
+        </is>
+      </c>
+      <c r="B1154" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:18:00</t>
+        </is>
+      </c>
+      <c r="B1155" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:19:00</t>
+        </is>
+      </c>
+      <c r="B1156" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:20:00</t>
+        </is>
+      </c>
+      <c r="B1157" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:21:00</t>
+        </is>
+      </c>
+      <c r="B1158" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:22:00</t>
+        </is>
+      </c>
+      <c r="B1159" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:23:00</t>
+        </is>
+      </c>
+      <c r="B1160" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:24:00</t>
+        </is>
+      </c>
+      <c r="B1161" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:25:00</t>
+        </is>
+      </c>
+      <c r="B1162" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>2025-09-14 15:26:00</t>
+        </is>
+      </c>
+      <c r="B1163" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" s="1" t="n">
+        <v>45914.57774482639</v>
+      </c>
+      <c r="B1164" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1164" t="n">
+        <v>550</v>
+      </c>
+      <c r="D1164" t="inlineStr">
+        <is>
+          <t>13:51</t>
+        </is>
+      </c>
+      <c r="E1164" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 550.0 MW/Tăng tải lên 550.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:24:00</t>
+        </is>
+      </c>
+      <c r="B1165" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:25:00</t>
+        </is>
+      </c>
+      <c r="B1166" t="n">
+        <v>442.2</v>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:26:00</t>
+        </is>
+      </c>
+      <c r="B1167" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:27:00</t>
+        </is>
+      </c>
+      <c r="B1168" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:28:00</t>
+        </is>
+      </c>
+      <c r="B1169" t="n">
+        <v>481.8</v>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:29:00</t>
+        </is>
+      </c>
+      <c r="B1170" t="n">
+        <v>494.9999999999999</v>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:30:00</t>
+        </is>
+      </c>
+      <c r="B1171" t="n">
+        <v>508.1999999999999</v>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:31:00</t>
+        </is>
+      </c>
+      <c r="B1172" t="n">
+        <v>521.4</v>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:32:00</t>
+        </is>
+      </c>
+      <c r="B1173" t="n">
+        <v>534.6</v>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:33:00</t>
+        </is>
+      </c>
+      <c r="B1174" t="n">
+        <v>547.8000000000001</v>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:34:00</t>
+        </is>
+      </c>
+      <c r="B1175" t="n">
+        <v>561.0000000000001</v>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:35:00</t>
+        </is>
+      </c>
+      <c r="B1176" t="n">
+        <v>574.2000000000002</v>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:36:00</t>
+        </is>
+      </c>
+      <c r="B1177" t="n">
+        <v>587.4000000000002</v>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:37:00</t>
+        </is>
+      </c>
+      <c r="B1178" t="n">
+        <v>600.6000000000003</v>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:38:00</t>
+        </is>
+      </c>
+      <c r="B1179" t="n">
+        <v>613.8000000000003</v>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:39:00</t>
+        </is>
+      </c>
+      <c r="B1180" t="n">
+        <v>627.0000000000003</v>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:40:00</t>
+        </is>
+      </c>
+      <c r="B1181" t="n">
+        <v>640.2000000000004</v>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:41:00</t>
+        </is>
+      </c>
+      <c r="B1182" t="n">
+        <v>653.4000000000004</v>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>2025-09-14 14:42:00</t>
+        </is>
+      </c>
+      <c r="B1183" t="n">
+        <v>660</v>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" s="1" t="n">
+        <v>45914.5796558912</v>
+      </c>
+      <c r="B1184" t="n">
+        <v>660</v>
+      </c>
+      <c r="C1184" t="n">
+        <v>264</v>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>13:54</t>
+        </is>
+      </c>
+      <c r="E1184" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" s="1" t="n">
+        <v>45914.58142091435</v>
+      </c>
+      <c r="B1185" t="n">
+        <v>660</v>
+      </c>
+      <c r="C1185" t="n">
+        <v>264</v>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
+      <c r="E1185" t="inlineStr">
+        <is>
+          <t>Decrease Unit load to 264.0 MW/Giảm tải xuống 264.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" s="1" t="n">
+        <v>45914.58549527778</v>
+      </c>
+      <c r="B1186" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1186" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>14:03</t>
+        </is>
+      </c>
+      <c r="E1186" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" s="1" t="n">
+        <v>45914.58573965278</v>
+      </c>
+      <c r="B1187" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1187" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>14:03</t>
+        </is>
+      </c>
+      <c r="E1187" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" s="1" t="n">
+        <v>45914.58614173611</v>
+      </c>
+      <c r="B1188" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1188" t="n">
+        <v>660</v>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>14:04</t>
+        </is>
+      </c>
+      <c r="E1188" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" s="1" t="n">
+        <v>45914.58711096065</v>
+      </c>
+      <c r="B1189" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1189" t="n">
+        <v>660</v>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>14:05</t>
+        </is>
+      </c>
+      <c r="E1189" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 660.0 MW/Tăng tải lên 660.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" s="1" t="n">
+        <v>45915.39805489562</v>
+      </c>
+      <c r="B1190" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1190" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="E1190" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:51:00</t>
+        </is>
+      </c>
+      <c r="B1191" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:52:00</t>
+        </is>
+      </c>
+      <c r="B1192" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:53:00</t>
+        </is>
+      </c>
+      <c r="B1193" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:54:00</t>
+        </is>
+      </c>
+      <c r="B1194" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:55:00</t>
+        </is>
+      </c>
+      <c r="B1195" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:56:00</t>
+        </is>
+      </c>
+      <c r="B1196" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:57:00</t>
+        </is>
+      </c>
+      <c r="B1197" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:58:00</t>
+        </is>
+      </c>
+      <c r="B1198" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:59:00</t>
+        </is>
+      </c>
+      <c r="B1199" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:00:00</t>
+        </is>
+      </c>
+      <c r="B1200" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:01:00</t>
+        </is>
+      </c>
+      <c r="B1201" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:02:00</t>
+        </is>
+      </c>
+      <c r="B1202" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:03:00</t>
+        </is>
+      </c>
+      <c r="B1203" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:04:00</t>
+        </is>
+      </c>
+      <c r="B1204" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:05:00</t>
+        </is>
+      </c>
+      <c r="B1205" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:06:00</t>
+        </is>
+      </c>
+      <c r="B1206" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:07:00</t>
+        </is>
+      </c>
+      <c r="B1207" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:08:00</t>
+        </is>
+      </c>
+      <c r="B1208" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" s="1" t="n">
+        <v>45915.39834450345</v>
+      </c>
+      <c r="B1209" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1209" t="n">
+        <v>600</v>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>09:33</t>
+        </is>
+      </c>
+      <c r="E1209" t="inlineStr">
+        <is>
+          <t>Increase Unit load to 600.0 MW/Tăng tải lên 600.0 MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:51:00</t>
+        </is>
+      </c>
+      <c r="B1210" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:52:00</t>
+        </is>
+      </c>
+      <c r="B1211" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:53:00</t>
+        </is>
+      </c>
+      <c r="B1212" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:54:00</t>
+        </is>
+      </c>
+      <c r="B1213" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:55:00</t>
+        </is>
+      </c>
+      <c r="B1214" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:56:00</t>
+        </is>
+      </c>
+      <c r="B1215" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:57:00</t>
+        </is>
+      </c>
+      <c r="B1216" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:58:00</t>
+        </is>
+      </c>
+      <c r="B1217" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:59:00</t>
+        </is>
+      </c>
+      <c r="B1218" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:00:00</t>
+        </is>
+      </c>
+      <c r="B1219" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:01:00</t>
+        </is>
+      </c>
+      <c r="B1220" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:02:00</t>
+        </is>
+      </c>
+      <c r="B1221" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:03:00</t>
+        </is>
+      </c>
+      <c r="B1222" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:04:00</t>
+        </is>
+      </c>
+      <c r="B1223" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:05:00</t>
+        </is>
+      </c>
+      <c r="B1224" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:06:00</t>
+        </is>
+      </c>
+      <c r="B1225" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:07:00</t>
+        </is>
+      </c>
+      <c r="B1226" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:08:00</t>
+        </is>
+      </c>
+      <c r="B1227" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:51:00</t>
+        </is>
+      </c>
+      <c r="B1228" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:52:00</t>
+        </is>
+      </c>
+      <c r="B1229" t="n">
+        <v>415.8</v>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:53:00</t>
+        </is>
+      </c>
+      <c r="B1230" t="n">
+        <v>402.6</v>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:54:00</t>
+        </is>
+      </c>
+      <c r="B1231" t="n">
+        <v>389.4</v>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:55:00</t>
+        </is>
+      </c>
+      <c r="B1232" t="n">
+        <v>376.2</v>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:56:00</t>
+        </is>
+      </c>
+      <c r="B1233" t="n">
+        <v>363.0000000000001</v>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:57:00</t>
+        </is>
+      </c>
+      <c r="B1234" t="n">
+        <v>349.8000000000001</v>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:58:00</t>
+        </is>
+      </c>
+      <c r="B1235" t="n">
+        <v>336.6000000000001</v>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>2025-09-15 10:59:00</t>
+        </is>
+      </c>
+      <c r="B1236" t="n">
+        <v>323.4000000000001</v>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:00:00</t>
+        </is>
+      </c>
+      <c r="B1237" t="n">
+        <v>316.8000000000001</v>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:01:00</t>
+        </is>
+      </c>
+      <c r="B1238" t="n">
+        <v>310.2</v>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:02:00</t>
+        </is>
+      </c>
+      <c r="B1239" t="n">
+        <v>303.6</v>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:03:00</t>
+        </is>
+      </c>
+      <c r="B1240" t="n">
+        <v>297</v>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:04:00</t>
+        </is>
+      </c>
+      <c r="B1241" t="n">
+        <v>290.4</v>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:05:00</t>
+        </is>
+      </c>
+      <c r="B1242" t="n">
+        <v>283.8</v>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:06:00</t>
+        </is>
+      </c>
+      <c r="B1243" t="n">
+        <v>277.1999999999999</v>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:07:00</t>
+        </is>
+      </c>
+      <c r="B1244" t="n">
+        <v>270.5999999999999</v>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:08:00</t>
+        </is>
+      </c>
+      <c r="B1245" t="n">
+        <v>264</v>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:08:00</t>
+        </is>
+      </c>
+      <c r="B1246" t="n">
+        <v>429</v>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:09:00</t>
+        </is>
+      </c>
+      <c r="B1247" t="n">
+        <v>442.2</v>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:10:00</t>
+        </is>
+      </c>
+      <c r="B1248" t="n">
+        <v>455.4</v>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:11:00</t>
+        </is>
+      </c>
+      <c r="B1249" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:12:00</t>
+        </is>
+      </c>
+      <c r="B1250" t="n">
+        <v>481.8</v>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:13:00</t>
+        </is>
+      </c>
+      <c r="B1251" t="n">
+        <v>494.9999999999999</v>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:14:00</t>
+        </is>
+      </c>
+      <c r="B1252" t="n">
+        <v>508.1999999999999</v>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:15:00</t>
+        </is>
+      </c>
+      <c r="B1253" t="n">
+        <v>521.4</v>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:16:00</t>
+        </is>
+      </c>
+      <c r="B1254" t="n">
+        <v>534.6</v>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:17:00</t>
+        </is>
+      </c>
+      <c r="B1255" t="n">
+        <v>547.8000000000001</v>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:18:00</t>
+        </is>
+      </c>
+      <c r="B1256" t="n">
+        <v>561.0000000000001</v>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:19:00</t>
+        </is>
+      </c>
+      <c r="B1257" t="n">
+        <v>574.2000000000002</v>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:20:00</t>
+        </is>
+      </c>
+      <c r="B1258" t="n">
+        <v>587.4000000000002</v>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:21:00</t>
+        </is>
+      </c>
+      <c r="B1259" t="n">
+        <v>600.6000000000003</v>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:22:00</t>
+        </is>
+      </c>
+      <c r="B1260" t="n">
+        <v>613.8000000000003</v>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:23:00</t>
+        </is>
+      </c>
+      <c r="B1261" t="n">
+        <v>627.0000000000003</v>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:24:00</t>
+        </is>
+      </c>
+      <c r="B1262" t="n">
+        <v>640.2000000000004</v>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:25:00</t>
+        </is>
+      </c>
+      <c r="B1263" t="n">
+        <v>653.4000000000004</v>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>ramp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>2025-09-15 11:26:00</t>
+        </is>
+      </c>
+      <c r="B1264" t="n">
+        <v>660</v>
+      </c>
+      <c r="C1264" t="inlineStr">
         <is>
           <t>ramp</t>
         </is>

</xml_diff>